<commit_message>
RX inversions corrected for cables 225834
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/vu13p.xlsx
+++ b/examples/vu13p_25g_all/src/vu13p.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vu13p_gty_refclk" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="vu13p_gty_inversions" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Instructions" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="vu13p_gty_inversions_non_inv_cables" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="vu13p_gty_inversions_inverted_cables" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Instructions" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="123">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -361,6 +362,12 @@
   </si>
   <si>
     <t xml:space="preserve">63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rx_invert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rx invert non-inverted cables</t>
   </si>
   <si>
     <t xml:space="preserve">Inversions map</t>
@@ -395,7 +402,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -417,6 +424,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -461,7 +474,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,6 +497,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1194,22 +1211,20 @@
   </sheetPr>
   <dimension ref="A1:D132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2763,6 +2778,2098 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E132"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="6" t="str">
+        <f aca="false">IF(E5="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="6" t="str">
+        <f aca="false">IF(E6="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="6" t="str">
+        <f aca="false">IF(E7="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f aca="false">IF(E8="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f aca="false">IF(E9="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="6" t="str">
+        <f aca="false">IF(E10="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6" t="str">
+        <f aca="false">IF(E11="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6" t="str">
+        <f aca="false">IF(E12="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6" t="str">
+        <f aca="false">IF(E13="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f aca="false">IF(E14="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6" t="str">
+        <f aca="false">IF(E15="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f aca="false">IF(E16="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f aca="false">IF(E17="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f aca="false">IF(E18="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6" t="str">
+        <f aca="false">IF(E19="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f aca="false">IF(E20="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="6" t="str">
+        <f aca="false">IF(E21="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="6" t="str">
+        <f aca="false">IF(E22="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="6" t="str">
+        <f aca="false">IF(E23="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="6" t="str">
+        <f aca="false">IF(E24="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="6" t="str">
+        <f aca="false">IF(E25="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="6" t="str">
+        <f aca="false">IF(E26="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="6" t="str">
+        <f aca="false">IF(E27="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="6" t="str">
+        <f aca="false">IF(E28="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="6" t="str">
+        <f aca="false">IF(E29="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="6" t="str">
+        <f aca="false">IF(E30="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="6" t="str">
+        <f aca="false">IF(E31="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="6" t="str">
+        <f aca="false">IF(E32="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="6" t="str">
+        <f aca="false">IF(E33="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="6" t="str">
+        <f aca="false">IF(E34="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="6" t="str">
+        <f aca="false">IF(E35="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="6" t="str">
+        <f aca="false">IF(E36="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="6" t="str">
+        <f aca="false">IF(E37="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="6" t="str">
+        <f aca="false">IF(E38="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="6" t="str">
+        <f aca="false">IF(E39="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="6" t="str">
+        <f aca="false">IF(E40="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="6" t="str">
+        <f aca="false">IF(E41="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="6" t="str">
+        <f aca="false">IF(E42="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="6" t="str">
+        <f aca="false">IF(E43="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="6" t="str">
+        <f aca="false">IF(E44="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="6" t="str">
+        <f aca="false">IF(E45="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="6" t="str">
+        <f aca="false">IF(E46="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="6" t="str">
+        <f aca="false">IF(E47="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="6" t="str">
+        <f aca="false">IF(E48="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="6" t="str">
+        <f aca="false">IF(E49="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="6" t="str">
+        <f aca="false">IF(E50="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="6" t="str">
+        <f aca="false">IF(E51="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="6" t="str">
+        <f aca="false">IF(E52="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" s="6" t="str">
+        <f aca="false">IF(E53="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="6" t="str">
+        <f aca="false">IF(E54="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="6" t="str">
+        <f aca="false">IF(E55="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="6" t="str">
+        <f aca="false">IF(E56="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="6" t="str">
+        <f aca="false">IF(E57="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="6" t="str">
+        <f aca="false">IF(E58="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="6" t="str">
+        <f aca="false">IF(E59="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="6" t="str">
+        <f aca="false">IF(E60="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="6" t="str">
+        <f aca="false">IF(E61="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="6" t="str">
+        <f aca="false">IF(E62="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="6" t="str">
+        <f aca="false">IF(E63="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="6" t="str">
+        <f aca="false">IF(E64="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="6" t="str">
+        <f aca="false">IF(E65="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="6" t="str">
+        <f aca="false">IF(E66="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67" s="6" t="str">
+        <f aca="false">IF(E67="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="6" t="str">
+        <f aca="false">IF(E68="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D69" s="6" t="str">
+        <f aca="false">IF(E69="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="6" t="str">
+        <f aca="false">IF(E70="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="6" t="str">
+        <f aca="false">IF(E71="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="6" t="str">
+        <f aca="false">IF(E72="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="6" t="str">
+        <f aca="false">IF(E73="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="6" t="str">
+        <f aca="false">IF(E74="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D75" s="6" t="str">
+        <f aca="false">IF(E75="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="6" t="str">
+        <f aca="false">IF(E76="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D77" s="6" t="str">
+        <f aca="false">IF(E77="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78" s="3"/>
+      <c r="D78" s="6" t="str">
+        <f aca="false">IF(E78="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D79" s="6" t="str">
+        <f aca="false">IF(E79="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="6" t="str">
+        <f aca="false">IF(E80="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="6" t="str">
+        <f aca="false">IF(E81="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" s="3"/>
+      <c r="D82" s="6" t="str">
+        <f aca="false">IF(E82="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D83" s="6" t="str">
+        <f aca="false">IF(E83="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="6" t="str">
+        <f aca="false">IF(E84="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C85" s="3"/>
+      <c r="D85" s="6" t="str">
+        <f aca="false">IF(E85="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="3"/>
+      <c r="D86" s="6" t="str">
+        <f aca="false">IF(E86="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C87" s="3"/>
+      <c r="D87" s="6" t="str">
+        <f aca="false">IF(E87="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C88" s="3"/>
+      <c r="D88" s="6" t="str">
+        <f aca="false">IF(E88="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C89" s="3"/>
+      <c r="D89" s="6" t="str">
+        <f aca="false">IF(E89="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C90" s="3"/>
+      <c r="D90" s="6" t="str">
+        <f aca="false">IF(E90="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="6" t="str">
+        <f aca="false">IF(E91="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="6" t="str">
+        <f aca="false">IF(E92="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C93" s="3"/>
+      <c r="D93" s="6" t="str">
+        <f aca="false">IF(E93="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C94" s="3"/>
+      <c r="D94" s="6" t="str">
+        <f aca="false">IF(E94="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="6" t="str">
+        <f aca="false">IF(E95="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C96" s="3"/>
+      <c r="D96" s="6" t="str">
+        <f aca="false">IF(E96="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="6" t="str">
+        <f aca="false">IF(E97="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C98" s="3"/>
+      <c r="D98" s="6" t="str">
+        <f aca="false">IF(E98="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="6" t="str">
+        <f aca="false">IF(E99="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C100" s="3"/>
+      <c r="D100" s="6" t="str">
+        <f aca="false">IF(E100="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="6" t="str">
+        <f aca="false">IF(E101="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C102" s="3"/>
+      <c r="D102" s="6" t="str">
+        <f aca="false">IF(E102="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C103" s="3"/>
+      <c r="D103" s="6" t="str">
+        <f aca="false">IF(E103="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104" s="3"/>
+      <c r="D104" s="6" t="str">
+        <f aca="false">IF(E104="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="6" t="str">
+        <f aca="false">IF(E105="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="6" t="str">
+        <f aca="false">IF(E106="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="6" t="str">
+        <f aca="false">IF(E107="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="6" t="str">
+        <f aca="false">IF(E108="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="6" t="str">
+        <f aca="false">IF(E109="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C110" s="3"/>
+      <c r="D110" s="6" t="str">
+        <f aca="false">IF(E110="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="6" t="str">
+        <f aca="false">IF(E111="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C112" s="3"/>
+      <c r="D112" s="6" t="str">
+        <f aca="false">IF(E112="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C113" s="3"/>
+      <c r="D113" s="6" t="str">
+        <f aca="false">IF(E113="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="6" t="str">
+        <f aca="false">IF(E114="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="6" t="str">
+        <f aca="false">IF(E115="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C116" s="3"/>
+      <c r="D116" s="6" t="str">
+        <f aca="false">IF(E116="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C117" s="3"/>
+      <c r="D117" s="6" t="str">
+        <f aca="false">IF(E117="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D118" s="6" t="str">
+        <f aca="false">IF(E118="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C119" s="3"/>
+      <c r="D119" s="6" t="str">
+        <f aca="false">IF(E119="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D120" s="6" t="str">
+        <f aca="false">IF(E120="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C121" s="3"/>
+      <c r="D121" s="6" t="str">
+        <f aca="false">IF(E121="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D122" s="6" t="str">
+        <f aca="false">IF(E122="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="6" t="str">
+        <f aca="false">IF(E123="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D124" s="6" t="str">
+        <f aca="false">IF(E124="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C125" s="3"/>
+      <c r="D125" s="6" t="str">
+        <f aca="false">IF(E125="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D126" s="6" t="str">
+        <f aca="false">IF(E126="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C127" s="3"/>
+      <c r="D127" s="6" t="str">
+        <f aca="false">IF(E127="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D128" s="6" t="str">
+        <f aca="false">IF(E128="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E128" s="3"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="6" t="str">
+        <f aca="false">IF(E129="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D130" s="6" t="str">
+        <f aca="false">IF(E130="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="6" t="str">
+        <f aca="false">IF(E131="x","","x")</f>
+        <v/>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D132" s="6" t="str">
+        <f aca="false">IF(E132="x","","x")</f>
+        <v>x</v>
+      </c>
+      <c r="E132" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2780,42 +4887,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected TXPOLARITY in X0Y4
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/vu13p.xlsx
+++ b/examples/vu13p_25g_all/src/vu13p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vu13p_gty_refclk" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="139">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -449,7 +449,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -478,12 +478,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -528,7 +522,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -559,10 +553,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -648,7 +638,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -1642,8 +1632,8 @@
   </sheetPr>
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1706,11 +1696,11 @@
         <v>66</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="8" t="str">
+      <c r="D5" s="2" t="str">
         <f aca="false">IF(E5="x","","x")</f>
         <v/>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1724,11 +1714,11 @@
       <c r="C6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="8" t="str">
+      <c r="D6" s="2" t="str">
         <f aca="false">IF(E6="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -1738,11 +1728,11 @@
         <v>69</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="8" t="str">
+      <c r="D7" s="2" t="str">
         <f aca="false">IF(E7="x","","x")</f>
         <v/>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1756,11 +1746,11 @@
       <c r="C8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="8" t="str">
+      <c r="D8" s="2" t="str">
         <f aca="false">IF(E8="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
@@ -1769,14 +1759,12 @@
       <c r="B9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="8" t="str">
+      <c r="C9" s="3"/>
+      <c r="D9" s="2" t="str">
         <f aca="false">IF(E9="x","","x")</f>
         <v/>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1790,11 +1778,11 @@
       <c r="C10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="8" t="str">
+      <c r="D10" s="2" t="str">
         <f aca="false">IF(E10="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
@@ -1804,11 +1792,11 @@
         <v>73</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="8" t="str">
+      <c r="D11" s="2" t="str">
         <f aca="false">IF(E11="x","","x")</f>
         <v/>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1820,11 +1808,11 @@
         <v>74</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="8" t="str">
+      <c r="D12" s="2" t="str">
         <f aca="false">IF(E12="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -1834,11 +1822,11 @@
         <v>75</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="8" t="str">
+      <c r="D13" s="2" t="str">
         <f aca="false">IF(E13="x","","x")</f>
         <v/>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1852,11 +1840,11 @@
       <c r="C14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="8" t="str">
+      <c r="D14" s="2" t="str">
         <f aca="false">IF(E14="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
@@ -1866,11 +1854,11 @@
         <v>77</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="8" t="str">
+      <c r="D15" s="2" t="str">
         <f aca="false">IF(E15="x","","x")</f>
         <v/>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1884,11 +1872,11 @@
       <c r="C16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="8" t="str">
+      <c r="D16" s="2" t="str">
         <f aca="false">IF(E16="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
@@ -1900,11 +1888,11 @@
       <c r="C17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="8" t="str">
+      <c r="D17" s="2" t="str">
         <f aca="false">IF(E17="x","","x")</f>
         <v/>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1918,11 +1906,11 @@
       <c r="C18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="8" t="str">
+      <c r="D18" s="2" t="str">
         <f aca="false">IF(E18="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
@@ -1932,11 +1920,11 @@
         <v>81</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="8" t="str">
+      <c r="D19" s="2" t="str">
         <f aca="false">IF(E19="x","","x")</f>
         <v/>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1950,11 +1938,11 @@
       <c r="C20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="8" t="str">
+      <c r="D20" s="2" t="str">
         <f aca="false">IF(E20="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
@@ -1964,11 +1952,11 @@
         <v>83</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="8" t="str">
+      <c r="D21" s="2" t="str">
         <f aca="false">IF(E21="x","","x")</f>
         <v/>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1980,11 +1968,11 @@
         <v>84</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="8" t="str">
+      <c r="D22" s="2" t="str">
         <f aca="false">IF(E22="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E22" s="9"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
@@ -1994,11 +1982,11 @@
         <v>85</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="8" t="str">
+      <c r="D23" s="2" t="str">
         <f aca="false">IF(E23="x","","x")</f>
         <v/>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2010,11 +1998,11 @@
         <v>86</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="8" t="str">
+      <c r="D24" s="2" t="str">
         <f aca="false">IF(E24="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
@@ -2024,11 +2012,11 @@
         <v>87</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="8" t="str">
+      <c r="D25" s="2" t="str">
         <f aca="false">IF(E25="x","","x")</f>
         <v/>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2040,11 +2028,11 @@
         <v>88</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="8" t="str">
+      <c r="D26" s="2" t="str">
         <f aca="false">IF(E26="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
@@ -2054,11 +2042,11 @@
         <v>89</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="8" t="str">
+      <c r="D27" s="2" t="str">
         <f aca="false">IF(E27="x","","x")</f>
         <v/>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2070,11 +2058,11 @@
         <v>90</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="8" t="str">
+      <c r="D28" s="2" t="str">
         <f aca="false">IF(E28="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E28" s="9"/>
+      <c r="E28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
@@ -2084,11 +2072,11 @@
         <v>91</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="8" t="str">
+      <c r="D29" s="2" t="str">
         <f aca="false">IF(E29="x","","x")</f>
         <v/>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2100,11 +2088,11 @@
         <v>92</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="8" t="str">
+      <c r="D30" s="2" t="str">
         <f aca="false">IF(E30="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
@@ -2114,11 +2102,11 @@
         <v>93</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="8" t="str">
+      <c r="D31" s="2" t="str">
         <f aca="false">IF(E31="x","","x")</f>
         <v/>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2130,11 +2118,11 @@
         <v>94</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="8" t="str">
+      <c r="D32" s="2" t="str">
         <f aca="false">IF(E32="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E32" s="9"/>
+      <c r="E32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
@@ -2144,11 +2132,11 @@
         <v>95</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="8" t="str">
+      <c r="D33" s="2" t="str">
         <f aca="false">IF(E33="x","","x")</f>
         <v/>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2160,11 +2148,11 @@
         <v>96</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="8" t="str">
+      <c r="D34" s="2" t="str">
         <f aca="false">IF(E34="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
@@ -2174,11 +2162,11 @@
         <v>97</v>
       </c>
       <c r="C35" s="3"/>
-      <c r="D35" s="8" t="str">
+      <c r="D35" s="2" t="str">
         <f aca="false">IF(E35="x","","x")</f>
         <v/>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2190,11 +2178,11 @@
         <v>98</v>
       </c>
       <c r="C36" s="3"/>
-      <c r="D36" s="8" t="str">
+      <c r="D36" s="2" t="str">
         <f aca="false">IF(E36="x","","x")</f>
         <v>x</v>
       </c>
-      <c r="E36" s="9"/>
+      <c r="E36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
@@ -2206,7 +2194,7 @@
       <c r="C37" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="8" t="str">
+      <c r="D37" s="2" t="str">
         <f aca="false">IF(E37="x","","x")</f>
         <v>x</v>
       </c>
@@ -2222,7 +2210,7 @@
       <c r="C38" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="8" t="str">
+      <c r="D38" s="2" t="str">
         <f aca="false">IF(E38="x","","x")</f>
         <v/>
       </c>
@@ -2240,7 +2228,7 @@
       <c r="C39" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="8" t="str">
+      <c r="D39" s="2" t="str">
         <f aca="false">IF(E39="x","","x")</f>
         <v>x</v>
       </c>
@@ -2256,7 +2244,7 @@
       <c r="C40" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="8" t="str">
+      <c r="D40" s="2" t="str">
         <f aca="false">IF(E40="x","","x")</f>
         <v/>
       </c>
@@ -2274,7 +2262,7 @@
       <c r="C41" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D41" s="8" t="str">
+      <c r="D41" s="2" t="str">
         <f aca="false">IF(E41="x","","x")</f>
         <v>x</v>
       </c>
@@ -2290,7 +2278,7 @@
       <c r="C42" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="8" t="str">
+      <c r="D42" s="2" t="str">
         <f aca="false">IF(E42="x","","x")</f>
         <v/>
       </c>
@@ -2308,7 +2296,7 @@
       <c r="C43" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="8" t="str">
+      <c r="D43" s="2" t="str">
         <f aca="false">IF(E43="x","","x")</f>
         <v>x</v>
       </c>
@@ -2324,7 +2312,7 @@
       <c r="C44" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="8" t="str">
+      <c r="D44" s="2" t="str">
         <f aca="false">IF(E44="x","","x")</f>
         <v/>
       </c>
@@ -2342,7 +2330,7 @@
       <c r="C45" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="8" t="str">
+      <c r="D45" s="2" t="str">
         <f aca="false">IF(E45="x","","x")</f>
         <v>x</v>
       </c>
@@ -2358,7 +2346,7 @@
       <c r="C46" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="8" t="str">
+      <c r="D46" s="2" t="str">
         <f aca="false">IF(E46="x","","x")</f>
         <v/>
       </c>
@@ -2376,7 +2364,7 @@
       <c r="C47" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="8" t="str">
+      <c r="D47" s="2" t="str">
         <f aca="false">IF(E47="x","","x")</f>
         <v>x</v>
       </c>
@@ -2392,7 +2380,7 @@
       <c r="C48" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="8" t="str">
+      <c r="D48" s="2" t="str">
         <f aca="false">IF(E48="x","","x")</f>
         <v/>
       </c>
@@ -2410,7 +2398,7 @@
       <c r="C49" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="8" t="str">
+      <c r="D49" s="2" t="str">
         <f aca="false">IF(E49="x","","x")</f>
         <v>x</v>
       </c>
@@ -2426,7 +2414,7 @@
       <c r="C50" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D50" s="8" t="str">
+      <c r="D50" s="2" t="str">
         <f aca="false">IF(E50="x","","x")</f>
         <v/>
       </c>
@@ -2444,7 +2432,7 @@
       <c r="C51" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D51" s="8" t="str">
+      <c r="D51" s="2" t="str">
         <f aca="false">IF(E51="x","","x")</f>
         <v>x</v>
       </c>
@@ -2460,7 +2448,7 @@
       <c r="C52" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D52" s="8" t="str">
+      <c r="D52" s="2" t="str">
         <f aca="false">IF(E52="x","","x")</f>
         <v/>
       </c>
@@ -2478,7 +2466,7 @@
       <c r="C53" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D53" s="8" t="str">
+      <c r="D53" s="2" t="str">
         <f aca="false">IF(E53="x","","x")</f>
         <v>x</v>
       </c>
@@ -2492,7 +2480,7 @@
         <v>116</v>
       </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="8" t="str">
+      <c r="D54" s="2" t="str">
         <f aca="false">IF(E54="x","","x")</f>
         <v/>
       </c>
@@ -2510,7 +2498,7 @@
       <c r="C55" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D55" s="8" t="str">
+      <c r="D55" s="2" t="str">
         <f aca="false">IF(E55="x","","x")</f>
         <v>x</v>
       </c>
@@ -2524,7 +2512,7 @@
         <v>118</v>
       </c>
       <c r="C56" s="3"/>
-      <c r="D56" s="8" t="str">
+      <c r="D56" s="2" t="str">
         <f aca="false">IF(E56="x","","x")</f>
         <v/>
       </c>
@@ -2542,7 +2530,7 @@
       <c r="C57" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D57" s="8" t="str">
+      <c r="D57" s="2" t="str">
         <f aca="false">IF(E57="x","","x")</f>
         <v>x</v>
       </c>
@@ -2556,7 +2544,7 @@
         <v>120</v>
       </c>
       <c r="C58" s="3"/>
-      <c r="D58" s="8" t="str">
+      <c r="D58" s="2" t="str">
         <f aca="false">IF(E58="x","","x")</f>
         <v/>
       </c>
@@ -2574,7 +2562,7 @@
       <c r="C59" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D59" s="8" t="str">
+      <c r="D59" s="2" t="str">
         <f aca="false">IF(E59="x","","x")</f>
         <v>x</v>
       </c>
@@ -2588,7 +2576,7 @@
         <v>122</v>
       </c>
       <c r="C60" s="3"/>
-      <c r="D60" s="8" t="str">
+      <c r="D60" s="2" t="str">
         <f aca="false">IF(E60="x","","x")</f>
         <v/>
       </c>
@@ -2606,7 +2594,7 @@
       <c r="C61" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="8" t="str">
+      <c r="D61" s="2" t="str">
         <f aca="false">IF(E61="x","","x")</f>
         <v>x</v>
       </c>
@@ -2620,7 +2608,7 @@
         <v>124</v>
       </c>
       <c r="C62" s="3"/>
-      <c r="D62" s="8" t="str">
+      <c r="D62" s="2" t="str">
         <f aca="false">IF(E62="x","","x")</f>
         <v/>
       </c>
@@ -2638,7 +2626,7 @@
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="8" t="str">
+      <c r="D63" s="2" t="str">
         <f aca="false">IF(E63="x","","x")</f>
         <v>x</v>
       </c>
@@ -2652,7 +2640,7 @@
         <v>126</v>
       </c>
       <c r="C64" s="3"/>
-      <c r="D64" s="8" t="str">
+      <c r="D64" s="2" t="str">
         <f aca="false">IF(E64="x","","x")</f>
         <v/>
       </c>
@@ -2670,7 +2658,7 @@
       <c r="C65" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D65" s="8" t="str">
+      <c r="D65" s="2" t="str">
         <f aca="false">IF(E65="x","","x")</f>
         <v>x</v>
       </c>
@@ -2684,7 +2672,7 @@
         <v>128</v>
       </c>
       <c r="C66" s="3"/>
-      <c r="D66" s="8" t="str">
+      <c r="D66" s="2" t="str">
         <f aca="false">IF(E66="x","","x")</f>
         <v/>
       </c>
@@ -2702,7 +2690,7 @@
       <c r="C67" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D67" s="8" t="str">
+      <c r="D67" s="2" t="str">
         <f aca="false">IF(E67="x","","x")</f>
         <v>x</v>
       </c>
@@ -2716,7 +2704,7 @@
         <v>130</v>
       </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="8" t="str">
+      <c r="D68" s="2" t="str">
         <f aca="false">IF(E68="x","","x")</f>
         <v/>
       </c>
@@ -2734,7 +2722,7 @@
       <c r="C69" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D69" s="8" t="str">
+      <c r="D69" s="2" t="str">
         <f aca="false">IF(E69="x","","x")</f>
         <v>x</v>
       </c>
@@ -2748,7 +2736,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="3"/>
-      <c r="D70" s="8" t="str">
+      <c r="D70" s="2" t="str">
         <f aca="false">IF(E70="x","","x")</f>
         <v/>
       </c>
@@ -2766,7 +2754,7 @@
       <c r="C71" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D71" s="8" t="str">
+      <c r="D71" s="2" t="str">
         <f aca="false">IF(E71="x","","x")</f>
         <v>x</v>
       </c>
@@ -2780,7 +2768,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="3"/>
-      <c r="D72" s="8" t="str">
+      <c r="D72" s="2" t="str">
         <f aca="false">IF(E72="x","","x")</f>
         <v/>
       </c>
@@ -2798,7 +2786,7 @@
       <c r="C73" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D73" s="8" t="str">
+      <c r="D73" s="2" t="str">
         <f aca="false">IF(E73="x","","x")</f>
         <v>x</v>
       </c>
@@ -2812,7 +2800,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="3"/>
-      <c r="D74" s="8" t="str">
+      <c r="D74" s="2" t="str">
         <f aca="false">IF(E74="x","","x")</f>
         <v/>
       </c>
@@ -2830,7 +2818,7 @@
       <c r="C75" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D75" s="8" t="str">
+      <c r="D75" s="2" t="str">
         <f aca="false">IF(E75="x","","x")</f>
         <v>x</v>
       </c>
@@ -2846,7 +2834,7 @@
       <c r="C76" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D76" s="8" t="str">
+      <c r="D76" s="2" t="str">
         <f aca="false">IF(E76="x","","x")</f>
         <v/>
       </c>
@@ -2864,7 +2852,7 @@
       <c r="C77" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D77" s="8" t="str">
+      <c r="D77" s="2" t="str">
         <f aca="false">IF(E77="x","","x")</f>
         <v>x</v>
       </c>
@@ -2878,7 +2866,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="3"/>
-      <c r="D78" s="8" t="str">
+      <c r="D78" s="2" t="str">
         <f aca="false">IF(E78="x","","x")</f>
         <v/>
       </c>
@@ -2896,7 +2884,7 @@
       <c r="C79" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D79" s="8" t="str">
+      <c r="D79" s="2" t="str">
         <f aca="false">IF(E79="x","","x")</f>
         <v>x</v>
       </c>
@@ -2910,7 +2898,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="3"/>
-      <c r="D80" s="8" t="str">
+      <c r="D80" s="2" t="str">
         <f aca="false">IF(E80="x","","x")</f>
         <v/>
       </c>
@@ -2926,7 +2914,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="3"/>
-      <c r="D81" s="8" t="str">
+      <c r="D81" s="2" t="str">
         <f aca="false">IF(E81="x","","x")</f>
         <v>x</v>
       </c>
@@ -2940,7 +2928,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="3"/>
-      <c r="D82" s="8" t="str">
+      <c r="D82" s="2" t="str">
         <f aca="false">IF(E82="x","","x")</f>
         <v/>
       </c>
@@ -2958,7 +2946,7 @@
       <c r="C83" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D83" s="8" t="str">
+      <c r="D83" s="2" t="str">
         <f aca="false">IF(E83="x","","x")</f>
         <v>x</v>
       </c>
@@ -2972,7 +2960,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="3"/>
-      <c r="D84" s="8" t="str">
+      <c r="D84" s="2" t="str">
         <f aca="false">IF(E84="x","","x")</f>
         <v/>
       </c>
@@ -2988,7 +2976,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="3"/>
-      <c r="D85" s="8" t="str">
+      <c r="D85" s="2" t="str">
         <f aca="false">IF(E85="x","","x")</f>
         <v>x</v>
       </c>
@@ -3002,7 +2990,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="3"/>
-      <c r="D86" s="8" t="str">
+      <c r="D86" s="2" t="str">
         <f aca="false">IF(E86="x","","x")</f>
         <v/>
       </c>
@@ -3018,7 +3006,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="3"/>
-      <c r="D87" s="8" t="str">
+      <c r="D87" s="2" t="str">
         <f aca="false">IF(E87="x","","x")</f>
         <v>x</v>
       </c>
@@ -3032,7 +3020,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="3"/>
-      <c r="D88" s="8" t="str">
+      <c r="D88" s="2" t="str">
         <f aca="false">IF(E88="x","","x")</f>
         <v/>
       </c>
@@ -3048,7 +3036,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="8" t="str">
+      <c r="D89" s="2" t="str">
         <f aca="false">IF(E89="x","","x")</f>
         <v>x</v>
       </c>
@@ -3062,7 +3050,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="3"/>
-      <c r="D90" s="8" t="str">
+      <c r="D90" s="2" t="str">
         <f aca="false">IF(E90="x","","x")</f>
         <v/>
       </c>
@@ -3078,7 +3066,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="3"/>
-      <c r="D91" s="8" t="str">
+      <c r="D91" s="2" t="str">
         <f aca="false">IF(E91="x","","x")</f>
         <v>x</v>
       </c>
@@ -3092,7 +3080,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="8" t="str">
+      <c r="D92" s="2" t="str">
         <f aca="false">IF(E92="x","","x")</f>
         <v/>
       </c>
@@ -3108,7 +3096,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="3"/>
-      <c r="D93" s="8" t="str">
+      <c r="D93" s="2" t="str">
         <f aca="false">IF(E93="x","","x")</f>
         <v>x</v>
       </c>
@@ -3122,7 +3110,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="3"/>
-      <c r="D94" s="8" t="str">
+      <c r="D94" s="2" t="str">
         <f aca="false">IF(E94="x","","x")</f>
         <v/>
       </c>
@@ -3138,7 +3126,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="3"/>
-      <c r="D95" s="8" t="str">
+      <c r="D95" s="2" t="str">
         <f aca="false">IF(E95="x","","x")</f>
         <v>x</v>
       </c>
@@ -3152,7 +3140,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="3"/>
-      <c r="D96" s="8" t="str">
+      <c r="D96" s="2" t="str">
         <f aca="false">IF(E96="x","","x")</f>
         <v/>
       </c>
@@ -3168,7 +3156,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="3"/>
-      <c r="D97" s="8" t="str">
+      <c r="D97" s="2" t="str">
         <f aca="false">IF(E97="x","","x")</f>
         <v>x</v>
       </c>
@@ -3182,7 +3170,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="3"/>
-      <c r="D98" s="8" t="str">
+      <c r="D98" s="2" t="str">
         <f aca="false">IF(E98="x","","x")</f>
         <v/>
       </c>
@@ -3198,7 +3186,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="3"/>
-      <c r="D99" s="8" t="str">
+      <c r="D99" s="2" t="str">
         <f aca="false">IF(E99="x","","x")</f>
         <v>x</v>
       </c>
@@ -3212,7 +3200,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="3"/>
-      <c r="D100" s="8" t="str">
+      <c r="D100" s="2" t="str">
         <f aca="false">IF(E100="x","","x")</f>
         <v/>
       </c>
@@ -3228,7 +3216,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="3"/>
-      <c r="D101" s="8" t="str">
+      <c r="D101" s="2" t="str">
         <f aca="false">IF(E101="x","","x")</f>
         <v/>
       </c>
@@ -3244,7 +3232,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="3"/>
-      <c r="D102" s="8" t="str">
+      <c r="D102" s="2" t="str">
         <f aca="false">IF(E102="x","","x")</f>
         <v>x</v>
       </c>
@@ -3258,7 +3246,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="3"/>
-      <c r="D103" s="8" t="str">
+      <c r="D103" s="2" t="str">
         <f aca="false">IF(E103="x","","x")</f>
         <v/>
       </c>
@@ -3274,7 +3262,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="3"/>
-      <c r="D104" s="8" t="str">
+      <c r="D104" s="2" t="str">
         <f aca="false">IF(E104="x","","x")</f>
         <v>x</v>
       </c>
@@ -3288,7 +3276,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="3"/>
-      <c r="D105" s="8" t="str">
+      <c r="D105" s="2" t="str">
         <f aca="false">IF(E105="x","","x")</f>
         <v/>
       </c>
@@ -3304,7 +3292,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="3"/>
-      <c r="D106" s="8" t="str">
+      <c r="D106" s="2" t="str">
         <f aca="false">IF(E106="x","","x")</f>
         <v>x</v>
       </c>
@@ -3318,7 +3306,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="3"/>
-      <c r="D107" s="8" t="str">
+      <c r="D107" s="2" t="str">
         <f aca="false">IF(E107="x","","x")</f>
         <v/>
       </c>
@@ -3334,7 +3322,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="3"/>
-      <c r="D108" s="8" t="str">
+      <c r="D108" s="2" t="str">
         <f aca="false">IF(E108="x","","x")</f>
         <v>x</v>
       </c>
@@ -3348,7 +3336,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="3"/>
-      <c r="D109" s="8" t="str">
+      <c r="D109" s="2" t="str">
         <f aca="false">IF(E109="x","","x")</f>
         <v/>
       </c>
@@ -3364,7 +3352,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="8" t="str">
+      <c r="D110" s="2" t="str">
         <f aca="false">IF(E110="x","","x")</f>
         <v>x</v>
       </c>
@@ -3378,7 +3366,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="3"/>
-      <c r="D111" s="8" t="str">
+      <c r="D111" s="2" t="str">
         <f aca="false">IF(E111="x","","x")</f>
         <v/>
       </c>
@@ -3394,7 +3382,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="3"/>
-      <c r="D112" s="8" t="str">
+      <c r="D112" s="2" t="str">
         <f aca="false">IF(E112="x","","x")</f>
         <v>x</v>
       </c>
@@ -3408,7 +3396,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="3"/>
-      <c r="D113" s="8" t="str">
+      <c r="D113" s="2" t="str">
         <f aca="false">IF(E113="x","","x")</f>
         <v/>
       </c>
@@ -3424,7 +3412,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="3"/>
-      <c r="D114" s="8" t="str">
+      <c r="D114" s="2" t="str">
         <f aca="false">IF(E114="x","","x")</f>
         <v>x</v>
       </c>
@@ -3438,7 +3426,7 @@
         <v>113</v>
       </c>
       <c r="C115" s="3"/>
-      <c r="D115" s="8" t="str">
+      <c r="D115" s="2" t="str">
         <f aca="false">IF(E115="x","","x")</f>
         <v/>
       </c>
@@ -3454,7 +3442,7 @@
         <v>114</v>
       </c>
       <c r="C116" s="3"/>
-      <c r="D116" s="8" t="str">
+      <c r="D116" s="2" t="str">
         <f aca="false">IF(E116="x","","x")</f>
         <v>x</v>
       </c>
@@ -3468,7 +3456,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="3"/>
-      <c r="D117" s="8" t="str">
+      <c r="D117" s="2" t="str">
         <f aca="false">IF(E117="x","","x")</f>
         <v/>
       </c>
@@ -3486,7 +3474,7 @@
       <c r="C118" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D118" s="8" t="str">
+      <c r="D118" s="2" t="str">
         <f aca="false">IF(E118="x","","x")</f>
         <v>x</v>
       </c>
@@ -3500,7 +3488,7 @@
         <v>117</v>
       </c>
       <c r="C119" s="3"/>
-      <c r="D119" s="8" t="str">
+      <c r="D119" s="2" t="str">
         <f aca="false">IF(E119="x","","x")</f>
         <v/>
       </c>
@@ -3518,7 +3506,7 @@
       <c r="C120" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D120" s="8" t="str">
+      <c r="D120" s="2" t="str">
         <f aca="false">IF(E120="x","","x")</f>
         <v>x</v>
       </c>
@@ -3532,7 +3520,7 @@
         <v>119</v>
       </c>
       <c r="C121" s="3"/>
-      <c r="D121" s="8" t="str">
+      <c r="D121" s="2" t="str">
         <f aca="false">IF(E121="x","","x")</f>
         <v/>
       </c>
@@ -3550,7 +3538,7 @@
       <c r="C122" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D122" s="8" t="str">
+      <c r="D122" s="2" t="str">
         <f aca="false">IF(E122="x","","x")</f>
         <v>x</v>
       </c>
@@ -3564,7 +3552,7 @@
         <v>121</v>
       </c>
       <c r="C123" s="3"/>
-      <c r="D123" s="8" t="str">
+      <c r="D123" s="2" t="str">
         <f aca="false">IF(E123="x","","x")</f>
         <v/>
       </c>
@@ -3582,7 +3570,7 @@
       <c r="C124" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D124" s="8" t="str">
+      <c r="D124" s="2" t="str">
         <f aca="false">IF(E124="x","","x")</f>
         <v>x</v>
       </c>
@@ -3596,7 +3584,7 @@
         <v>123</v>
       </c>
       <c r="C125" s="3"/>
-      <c r="D125" s="8" t="str">
+      <c r="D125" s="2" t="str">
         <f aca="false">IF(E125="x","","x")</f>
         <v/>
       </c>
@@ -3614,7 +3602,7 @@
       <c r="C126" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D126" s="8" t="str">
+      <c r="D126" s="2" t="str">
         <f aca="false">IF(E126="x","","x")</f>
         <v>x</v>
       </c>
@@ -3628,7 +3616,7 @@
         <v>125</v>
       </c>
       <c r="C127" s="3"/>
-      <c r="D127" s="8" t="str">
+      <c r="D127" s="2" t="str">
         <f aca="false">IF(E127="x","","x")</f>
         <v/>
       </c>
@@ -3646,7 +3634,7 @@
       <c r="C128" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D128" s="8" t="str">
+      <c r="D128" s="2" t="str">
         <f aca="false">IF(E128="x","","x")</f>
         <v>x</v>
       </c>
@@ -3660,7 +3648,7 @@
         <v>127</v>
       </c>
       <c r="C129" s="3"/>
-      <c r="D129" s="8" t="str">
+      <c r="D129" s="2" t="str">
         <f aca="false">IF(E129="x","","x")</f>
         <v/>
       </c>
@@ -3678,7 +3666,7 @@
       <c r="C130" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D130" s="8" t="str">
+      <c r="D130" s="2" t="str">
         <f aca="false">IF(E130="x","","x")</f>
         <v>x</v>
       </c>
@@ -3692,7 +3680,7 @@
         <v>129</v>
       </c>
       <c r="C131" s="3"/>
-      <c r="D131" s="8" t="str">
+      <c r="D131" s="2" t="str">
         <f aca="false">IF(E131="x","","x")</f>
         <v/>
       </c>
@@ -3710,7 +3698,7 @@
       <c r="C132" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D132" s="8" t="str">
+      <c r="D132" s="2" t="str">
         <f aca="false">IF(E132="x","","x")</f>
         <v>x</v>
       </c>

</xml_diff>

<commit_message>
complete link map for phaseII EMTF done, SV generated
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/vu13p.xlsx
+++ b/examples/vu13p_25g_all/src/vu13p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="vu13p_gty_refclk" sheetId="1" state="visible" r:id="rId2"/>
@@ -153,7 +153,7 @@
     <t xml:space="preserve">J11</t>
   </si>
   <si>
-    <t xml:space="preserve">160.32</t>
+    <t xml:space="preserve">320.64</t>
   </si>
   <si>
     <t xml:space="preserve">BA41</t>
@@ -638,8 +638,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1632,8 +1632,8 @@
   </sheetPr>
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="C37:C52 C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3723,7 +3723,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="C37:C52 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>